<commit_message>
Working Model No Sup
This is a full working model, in order to use it at this point I would need to add the hatchery and supplementation scenarios.
</commit_message>
<xml_diff>
--- a/UGR_LifeCycleInput.xlsx
+++ b/UGR_LifeCycleInput.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21700" yWindow="680" windowWidth="26480" windowHeight="23880" activeTab="1" xr2:uid="{BDC6114A-2371-C44B-9A16-408EBE939B3C}"/>
+    <workbookView xWindow="29460" yWindow="620" windowWidth="25440" windowHeight="23420" activeTab="1" xr2:uid="{BDC6114A-2371-C44B-9A16-408EBE939B3C}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelHeader" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>Description</t>
   </si>
@@ -137,13 +137,22 @@
   </si>
   <si>
     <t>Capacity_SD</t>
+  </si>
+  <si>
+    <t>Spawner1Egg</t>
+  </si>
+  <si>
+    <t>Spawner2Egg</t>
+  </si>
+  <si>
+    <t>Spawner3Egg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -167,13 +176,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -185,10 +218,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -197,8 +232,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -573,13 +616,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F84DFF48-A062-124A-A02D-23ED0D7E0F71}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -630,10 +673,10 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="2" t="str">
@@ -647,7 +690,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>100000000</v>
+        <v>1E+20</v>
       </c>
       <c r="G2" s="2">
         <v>0</v>
@@ -659,21 +702,21 @@
         <v>0</v>
       </c>
       <c r="J2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="2" t="str">
-        <f t="shared" ref="C3:C20" si="0">A3&amp;"_"&amp;B3</f>
+        <f t="shared" ref="C3:C21" si="0">A3&amp;"_"&amp;B3</f>
         <v>Fry_Parr</v>
       </c>
       <c r="D3" s="2">
@@ -683,7 +726,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2">
-        <v>100000000</v>
+        <v>1E+20</v>
       </c>
       <c r="G3" s="2">
         <v>0</v>
@@ -702,10 +745,10 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="2" t="str">
@@ -719,7 +762,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="2">
-        <v>100000000</v>
+        <v>1E+20</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
@@ -738,10 +781,10 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="2" t="str">
@@ -755,7 +798,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>100000000</v>
+        <v>1E+20</v>
       </c>
       <c r="G5" s="2">
         <v>0</v>
@@ -774,10 +817,10 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="2" t="str">
@@ -791,7 +834,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>100000000</v>
+        <v>1E+20</v>
       </c>
       <c r="G6" s="2">
         <v>0</v>
@@ -810,10 +853,10 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="2" t="str">
@@ -827,7 +870,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="2">
-        <v>100000000</v>
+        <v>1E+20</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
@@ -846,10 +889,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="2" t="str">
@@ -863,13 +906,13 @@
         <v>0</v>
       </c>
       <c r="F8" s="2">
-        <v>100000000</v>
+        <v>1E+20</v>
       </c>
       <c r="G8" s="2">
         <v>0</v>
       </c>
       <c r="H8" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I8" s="2">
         <v>0</v>
@@ -882,52 +925,52 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>LGDSmolt_OceanAdult1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1E+20</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>2</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="2" t="str">
+      <c r="C10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OceanAdult1_LGDAdult2</v>
       </c>
-      <c r="D9" s="2">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>100000000</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2">
-        <v>1</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2">
-        <v>3</v>
-      </c>
-      <c r="K9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>OceanAdult1_OceanAdult2</v>
-      </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
@@ -935,13 +978,13 @@
         <v>0</v>
       </c>
       <c r="F10" s="2">
-        <v>100000000</v>
+        <v>1E+20</v>
       </c>
       <c r="G10" s="2">
         <v>0</v>
       </c>
       <c r="H10" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I10" s="2">
         <v>0</v>
@@ -954,362 +997,398 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>OceanAdult1_OceanAdult2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1E+20</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>3</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="2" t="str">
+      <c r="C12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OceanAdult2_LGDAdult3</v>
       </c>
-      <c r="D11" s="2">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>100000000</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2">
-        <v>1</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2">
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1E+20</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
         <v>4</v>
       </c>
-      <c r="K11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="2" t="str">
+      <c r="C13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>LGDAdult1_TrapAdult1</v>
       </c>
-      <c r="D12" s="2">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>100000000</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0</v>
-      </c>
-      <c r="H12" s="2">
-        <v>1</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1E+20</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
         <v>2</v>
       </c>
-      <c r="K12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="2" t="str">
+      <c r="C14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>LGDAdult2_TrapAdult2</v>
       </c>
-      <c r="D13" s="2">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>100000000</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2">
-        <v>1</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2">
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1E+20</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
         <v>3</v>
       </c>
-      <c r="K13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="2" t="str">
+      <c r="C15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>LGDAdult3_TrapAdult3</v>
       </c>
-      <c r="D14" s="2">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2">
-        <v>100000000</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2">
-        <v>1</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1E+20</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
         <v>4</v>
       </c>
-      <c r="K14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="2" t="str">
+      <c r="C16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>TrapAdult1_Spawner1</v>
       </c>
-      <c r="D15" s="2">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2">
-        <v>100000000</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2">
-        <v>1</v>
-      </c>
-      <c r="I15" s="2">
-        <v>0</v>
-      </c>
-      <c r="J15" s="2">
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1E+20</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
         <v>2</v>
       </c>
-      <c r="K15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="K16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="2" t="str">
+      <c r="C17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>TrapAdult2_Spawner2</v>
       </c>
-      <c r="D16" s="2">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>100000000</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0</v>
-      </c>
-      <c r="H16" s="2">
-        <v>1</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0</v>
-      </c>
-      <c r="J16" s="2">
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1E+20</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
         <v>3</v>
       </c>
-      <c r="K16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="K17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="2" t="str">
+      <c r="C18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>TrapAdult3_Spawner3</v>
       </c>
-      <c r="D17" s="2">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2">
-        <v>100000000</v>
-      </c>
-      <c r="G17" s="2">
-        <v>0</v>
-      </c>
-      <c r="H17" s="2">
-        <v>1</v>
-      </c>
-      <c r="I17" s="2">
-        <v>0</v>
-      </c>
-      <c r="J17" s="2">
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1E+20</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
         <v>4</v>
       </c>
-      <c r="K17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Spawner1_Egg</v>
-      </c>
-      <c r="D18" s="2">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2">
-        <v>100000000</v>
-      </c>
-      <c r="G18" s="2">
-        <v>0</v>
-      </c>
-      <c r="H18" s="2">
-        <v>1</v>
-      </c>
-      <c r="I18" s="2">
-        <v>0</v>
-      </c>
-      <c r="J18" s="2">
+      <c r="B19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Spawner1_Spawner1Egg</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1E+20</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2">
         <v>2</v>
       </c>
-      <c r="K18" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Spawner2_Egg</v>
-      </c>
-      <c r="D19" s="2">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2">
-        <v>100000000</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0</v>
-      </c>
-      <c r="H19" s="2">
-        <v>1</v>
-      </c>
-      <c r="I19" s="2">
-        <v>0</v>
-      </c>
-      <c r="J19" s="2">
+      <c r="B20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Spawner2_Spawner2Egg</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1E+20</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
         <v>3</v>
       </c>
-      <c r="K19" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Spawner3_Egg</v>
-      </c>
-      <c r="D20" s="2">
-        <v>1</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0</v>
-      </c>
-      <c r="F20" s="2">
-        <v>100000000</v>
-      </c>
-      <c r="G20" s="2">
-        <v>0</v>
-      </c>
-      <c r="H20" s="2">
-        <v>1</v>
-      </c>
-      <c r="I20" s="2">
-        <v>0</v>
-      </c>
-      <c r="J20" s="2">
+      <c r="B21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Spawner3_Spawner3Egg</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1E+20</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
         <v>4</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K21" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Just before adding hatchery scaler
Updated the Bev Holt to use a hatchery scaler, gonna be a hitch
</commit_message>
<xml_diff>
--- a/UGR_LifeCycleInput.xlsx
+++ b/UGR_LifeCycleInput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Documents/NicksSoftware/UGR_LCM_Weber/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157C9AEA-883F-1945-B70A-640B29666201}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F841762F-2DD0-D845-B0B5-B0DE07DD3770}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2040" windowWidth="32120" windowHeight="25380" activeTab="1" xr2:uid="{BDC6114A-2371-C44B-9A16-408EBE939B3C}"/>
+    <workbookView xWindow="1240" yWindow="780" windowWidth="24620" windowHeight="25420" activeTab="1" xr2:uid="{BDC6114A-2371-C44B-9A16-408EBE939B3C}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelHeader" sheetId="2" r:id="rId1"/>
@@ -743,7 +743,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -828,16 +828,16 @@
         <v>Fry_Parr</v>
       </c>
       <c r="D3" s="2">
-        <v>0.23</v>
+        <v>0.15</v>
       </c>
       <c r="E3" s="2">
-        <v>1E-3</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="F3" s="6">
         <v>165687.37610977169</v>
       </c>
       <c r="G3" s="2">
-        <v>0</v>
+        <v>22359</v>
       </c>
       <c r="H3" s="2">
         <v>1</v>
@@ -870,7 +870,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2">
-        <v>0.5</v>
+        <v>0.23</v>
       </c>
       <c r="I4" s="2">
         <v>0</v>
@@ -900,7 +900,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2">
-        <v>0.5</v>
+        <v>0.77</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
@@ -921,7 +921,7 @@
         <v>0.11</v>
       </c>
       <c r="E6" s="2">
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
       <c r="F6" s="2">
         <v>1E+20</v>
@@ -951,7 +951,7 @@
         <v>0.13</v>
       </c>
       <c r="E7" s="2">
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
       <c r="F7" s="2">
         <v>1E+20</v>
@@ -978,16 +978,19 @@
         <v>HatchRelease_LGDSmolt</v>
       </c>
       <c r="D8" s="2">
-        <v>0.65</v>
+        <v>0.68</v>
       </c>
       <c r="E8" s="2">
-        <v>0.1</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F8" s="2">
         <v>1E+20</v>
       </c>
       <c r="G8" s="2">
         <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
       </c>
       <c r="I8" s="2">
         <v>0</v>
@@ -1005,10 +1008,10 @@
         <v>LGDSmolt_LGDAdult1</v>
       </c>
       <c r="D9" s="2">
-        <v>0.02</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="E9" s="2">
-        <v>1E-3</v>
+        <v>2.3E-2</v>
       </c>
       <c r="F9" s="2">
         <v>1E+20</v>
@@ -1017,7 +1020,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="2">
-        <v>0.113</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="I9" s="2">
         <v>0</v>
@@ -1035,10 +1038,10 @@
         <v>LGDSmolt_OceanAdult1</v>
       </c>
       <c r="D10" s="2">
-        <v>0.02</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="E10" s="2">
-        <v>1E-3</v>
+        <v>2.3E-2</v>
       </c>
       <c r="F10" s="2">
         <v>1E+20</v>
@@ -1047,7 +1050,8 @@
         <v>0</v>
       </c>
       <c r="H10" s="2">
-        <v>0.88700000000000001</v>
+        <f>1-H9</f>
+        <v>0.93100000000000005</v>
       </c>
       <c r="I10" s="2">
         <v>0</v>
@@ -1065,10 +1069,10 @@
         <v>OceanAdult1_LGDAdult2</v>
       </c>
       <c r="D11" s="2">
-        <v>0.318</v>
+        <v>0.24</v>
       </c>
       <c r="E11" s="2">
-        <v>0.01</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F11" s="2">
         <v>1E+20</v>
@@ -1077,7 +1081,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="2">
-        <v>0.95099999999999996</v>
+        <v>0.93</v>
       </c>
       <c r="I11" s="2">
         <v>0</v>
@@ -1095,10 +1099,10 @@
         <v>OceanAdult1_OceanAdult2</v>
       </c>
       <c r="D12" s="2">
-        <v>0.318</v>
+        <v>0.24</v>
       </c>
       <c r="E12" s="2">
-        <v>0.01</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F12" s="2">
         <v>1E+20</v>
@@ -1107,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="2">
-        <v>4.9000000000000002E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="I12" s="2">
         <v>0</v>
@@ -1125,10 +1129,10 @@
         <v>OceanAdult2_LGDAdult3</v>
       </c>
       <c r="D13" s="2">
-        <v>0.55600000000000005</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E13" s="2">
-        <v>0.01</v>
+        <v>2.3E-2</v>
       </c>
       <c r="F13" s="2">
         <v>1E+20</v>
@@ -1158,7 +1162,7 @@
         <v>0.9</v>
       </c>
       <c r="E14" s="2">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="F14" s="2">
         <v>1E+20</v>
@@ -1188,7 +1192,7 @@
         <v>0.97</v>
       </c>
       <c r="E15" s="2">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="F15" s="2">
         <v>1E+20</v>
@@ -1215,16 +1219,16 @@
         <v>Spawner_Egg</v>
       </c>
       <c r="D16" s="2">
-        <v>3257</v>
+        <v>3831</v>
       </c>
       <c r="E16" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>7370834.7000000002</v>
+        <v>49138898.203365818</v>
       </c>
       <c r="G16" s="2">
-        <v>1000</v>
+        <v>921</v>
       </c>
       <c r="H16" s="2">
         <v>1</v>

</xml_diff>